<commit_message>
updated page link in testcases
</commit_message>
<xml_diff>
--- a/docs/testCases/firstSprint/1.TestCase-Navigation.xlsx
+++ b/docs/testCases/firstSprint/1.TestCase-Navigation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projektas\StrangerTeam_PayApi_Project\docs\testCases\firstSprint\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276134DE-EE44-4172-979A-E1325BED37E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F03F2C-E2A4-4BA9-A107-E5FF72D773F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7320" yWindow="3525" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -105,9 +105,6 @@
     <t>As a site visitor, I want to be able to clearly see navigation options and sites logo.</t>
   </si>
   <si>
-    <t>Go to the web pagelink: https://stranger-team-project-61ydf6mit-jkilius-projects.vercel.app/</t>
-  </si>
-  <si>
     <t>Mobile</t>
   </si>
   <si>
@@ -139,6 +136,9 @@
   </si>
   <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>Go to the web pagelink: https://stranger-team-pay-api-project.vercel.app/</t>
   </si>
 </sst>
 </file>
@@ -327,13 +327,11 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -341,38 +339,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -387,6 +355,9 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -396,13 +367,42 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -687,23 +687,23 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="B20" sqref="B20:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
+      <c r="B1" s="23"/>
       <c r="C1" s="1">
         <v>1</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="14"/>
+      <c r="E1" s="23"/>
       <c r="F1" s="15" t="s">
         <v>24</v>
       </c>
@@ -714,25 +714,25 @@
       <c r="K1" s="16"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="14"/>
+      <c r="B2" s="23"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="14"/>
+      <c r="E2" s="23"/>
       <c r="F2" s="15"/>
       <c r="G2" s="16"/>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="14"/>
-      <c r="J2" s="18" t="s">
+      <c r="I2" s="23"/>
+      <c r="J2" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="19"/>
+      <c r="K2" s="34"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
@@ -748,10 +748,10 @@
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="21"/>
+      <c r="B4" s="36"/>
       <c r="C4" s="3"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -776,27 +776,27 @@
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="21"/>
+      <c r="B6" s="36"/>
       <c r="C6" s="5"/>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="21"/>
-      <c r="F6" s="22">
+      <c r="E6" s="36"/>
+      <c r="F6" s="37">
         <v>45267</v>
       </c>
-      <c r="G6" s="23"/>
-      <c r="H6" s="17" t="s">
+      <c r="G6" s="38"/>
+      <c r="H6" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="21"/>
-      <c r="J6" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="K6" s="12"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="K6" s="31"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
@@ -815,28 +815,28 @@
       <c r="A8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
       <c r="E8" s="7"/>
       <c r="F8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="30"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>1</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="14" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="15"/>
@@ -845,7 +845,7 @@
       <c r="F9" s="9">
         <v>1</v>
       </c>
-      <c r="G9" s="27"/>
+      <c r="G9" s="14"/>
       <c r="H9" s="15"/>
       <c r="I9" s="15"/>
       <c r="J9" s="15"/>
@@ -855,7 +855,7 @@
       <c r="A10" s="9">
         <v>2</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="14" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="15"/>
@@ -864,7 +864,7 @@
       <c r="F10" s="9">
         <v>2</v>
       </c>
-      <c r="G10" s="27"/>
+      <c r="G10" s="14"/>
       <c r="H10" s="15"/>
       <c r="I10" s="15"/>
       <c r="J10" s="15"/>
@@ -874,7 +874,7 @@
       <c r="A11" s="9">
         <v>3</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="14" t="s">
         <v>20</v>
       </c>
       <c r="C11" s="15"/>
@@ -883,7 +883,7 @@
       <c r="F11" s="9">
         <v>3</v>
       </c>
-      <c r="G11" s="27"/>
+      <c r="G11" s="14"/>
       <c r="H11" s="15"/>
       <c r="I11" s="15"/>
       <c r="J11" s="15"/>
@@ -893,7 +893,7 @@
       <c r="A12" s="9">
         <v>4</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="14" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="15"/>
@@ -902,7 +902,7 @@
       <c r="F12" s="9">
         <v>4</v>
       </c>
-      <c r="G12" s="27"/>
+      <c r="G12" s="14"/>
       <c r="H12" s="15"/>
       <c r="I12" s="15"/>
       <c r="J12" s="15"/>
@@ -912,7 +912,7 @@
       <c r="A13" s="9">
         <v>5</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="14" t="s">
         <v>22</v>
       </c>
       <c r="C13" s="15"/>
@@ -921,7 +921,7 @@
       <c r="F13" s="9">
         <v>5</v>
       </c>
-      <c r="G13" s="27"/>
+      <c r="G13" s="14"/>
       <c r="H13" s="15"/>
       <c r="I13" s="15"/>
       <c r="J13" s="15"/>
@@ -931,8 +931,8 @@
       <c r="A14" s="9">
         <v>6</v>
       </c>
-      <c r="B14" s="27" t="s">
-        <v>27</v>
+      <c r="B14" s="14" t="s">
+        <v>26</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="16"/>
@@ -940,7 +940,7 @@
       <c r="F14" s="9">
         <v>6</v>
       </c>
-      <c r="G14" s="27"/>
+      <c r="G14" s="14"/>
       <c r="H14" s="15"/>
       <c r="I14" s="15"/>
       <c r="J14" s="15"/>
@@ -950,14 +950,14 @@
       <c r="A16" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -977,60 +977,60 @@
       <c r="K17" s="11"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="29"/>
-      <c r="D18" s="31" t="s">
+      <c r="C18" s="19"/>
+      <c r="D18" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="32"/>
-      <c r="F18" s="28" t="s">
+      <c r="E18" s="22"/>
+      <c r="F18" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="28" t="s">
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="J18" s="33"/>
-      <c r="K18" s="33"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="29"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="33"/>
-      <c r="J19" s="33"/>
-      <c r="K19" s="33"/>
+      <c r="A19" s="19"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
     </row>
     <row r="20" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>1</v>
       </c>
-      <c r="B20" s="36" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="37"/>
-      <c r="D20" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="E20" s="36"/>
-      <c r="F20" s="27" t="s">
-        <v>36</v>
+      <c r="B20" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="17"/>
+      <c r="D20" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="12"/>
+      <c r="F20" s="14" t="s">
+        <v>35</v>
       </c>
       <c r="G20" s="15"/>
       <c r="H20" s="16"/>
-      <c r="I20" s="27" t="s">
-        <v>35</v>
+      <c r="I20" s="14" t="s">
+        <v>34</v>
       </c>
       <c r="J20" s="15"/>
       <c r="K20" s="16"/>
@@ -1039,21 +1039,21 @@
       <c r="A21" s="9">
         <v>2</v>
       </c>
-      <c r="B21" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="38"/>
-      <c r="D21" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="E21" s="36"/>
-      <c r="F21" s="27" t="s">
-        <v>36</v>
+      <c r="B21" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="13"/>
+      <c r="D21" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="12"/>
+      <c r="F21" s="14" t="s">
+        <v>35</v>
       </c>
       <c r="G21" s="15"/>
       <c r="H21" s="16"/>
-      <c r="I21" s="27" t="s">
-        <v>35</v>
+      <c r="I21" s="14" t="s">
+        <v>34</v>
       </c>
       <c r="J21" s="15"/>
       <c r="K21" s="16"/>
@@ -1062,21 +1062,21 @@
       <c r="A22" s="9">
         <v>3</v>
       </c>
-      <c r="B22" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="38"/>
-      <c r="D22" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="E22" s="36"/>
-      <c r="F22" s="27" t="s">
-        <v>36</v>
+      <c r="B22" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="13"/>
+      <c r="D22" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" s="12"/>
+      <c r="F22" s="14" t="s">
+        <v>35</v>
       </c>
       <c r="G22" s="15"/>
       <c r="H22" s="16"/>
-      <c r="I22" s="27" t="s">
-        <v>35</v>
+      <c r="I22" s="14" t="s">
+        <v>34</v>
       </c>
       <c r="J22" s="15"/>
       <c r="K22" s="16"/>
@@ -1085,63 +1085,27 @@
       <c r="A23" s="9">
         <v>4</v>
       </c>
-      <c r="B23" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="38"/>
-      <c r="D23" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="E23" s="36"/>
-      <c r="F23" s="27" t="s">
-        <v>36</v>
+      <c r="B23" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="13"/>
+      <c r="D23" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" s="12"/>
+      <c r="F23" s="14" t="s">
+        <v>35</v>
       </c>
       <c r="G23" s="15"/>
       <c r="H23" s="16"/>
-      <c r="I23" s="27" t="s">
-        <v>35</v>
+      <c r="I23" s="14" t="s">
+        <v>34</v>
       </c>
       <c r="J23" s="15"/>
       <c r="K23" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="G14:K14"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:C19"/>
-    <mergeCell ref="D18:E19"/>
-    <mergeCell ref="F18:H19"/>
-    <mergeCell ref="I18:K19"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="G11:K11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="G12:K12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="G13:K13"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="G9:K9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="G10:K10"/>
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
@@ -1156,6 +1120,42 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="H6:I6"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="G10:K10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="G11:K11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="G12:K12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="G13:K13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="G14:K14"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:C19"/>
+    <mergeCell ref="D18:E19"/>
+    <mergeCell ref="F18:H19"/>
+    <mergeCell ref="I18:K19"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="I23:K23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>